<commit_message>
configuracion de gastos comunes y no comunes en el sistema
</commit_message>
<xml_diff>
--- a/public/downloads/carga-de-viviendas.xlsx
+++ b/public/downloads/carga-de-viviendas.xlsx
@@ -16,19 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Ricardo</t>
-  </si>
-  <si>
-    <t>Belisario</t>
-  </si>
-  <si>
-    <t>ricardo@belisario</t>
-  </si>
-  <si>
-    <t>D-60</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Nombre0</t>
   </si>
@@ -398,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="C2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -411,66 +399,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>2122222222</v>
-      </c>
-      <c r="I2">
-        <v>4140000000</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>